<commit_message>
Updated user requirements. Removed VS specific files from tracking.
</commit_message>
<xml_diff>
--- a/SRS/requirements.xlsx
+++ b/SRS/requirements.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Logger" sheetId="1" r:id="rId1"/>
+    <sheet name="TI" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Status</t>
   </si>
@@ -50,6 +51,30 @@
   </si>
   <si>
     <t>LogMsg(string msg) - Automatically add timestamp to display. Format is "HH:MM:SS"</t>
+  </si>
+  <si>
+    <t>Trading Instrument Requirements</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>A list of available trading instruments shall be created from the app.config configuration file at startup. Invalid entries shall be ignored.</t>
+  </si>
+  <si>
+    <t>Available trading instruments shall automatically subscribe to real-time data after connection to the broker.</t>
+  </si>
+  <si>
+    <t>User Story</t>
+  </si>
+  <si>
+    <t>Trading data shall be stored in 1-minute increments for the last year for each available instrument. The High/Low/Open/Close for each interval shall be stored in a separate file.</t>
+  </si>
+  <si>
+    <t>Trading data shall be stored the following format: "TIMESTAMP,OPEN,CLOSE,HIGH,LOW". The timestamp shall be "MONTH/DAY/YEAR" with Month/Day as one or 2 digits and year as 4 digits.</t>
+  </si>
+  <si>
+    <t>Trading prices shall add zeros such that all data has the same string length (i.e: "1000.25,1005,1000.50,900,500.005" shall be coded as "1000.250,1005.000,1000.500,500.005"</t>
   </si>
 </sst>
 </file>
@@ -110,6 +135,21 @@
   <autoFilter ref="A2:D51"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Status"/>
+    <tableColumn id="2" name="Req#"/>
+    <tableColumn id="3" name="Category"/>
+    <tableColumn id="4" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A2:F49" totalsRowShown="0">
+  <autoFilter ref="A2:F49"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Status"/>
+    <tableColumn id="5" name="Priority"/>
+    <tableColumn id="6" name="User Story"/>
     <tableColumn id="2" name="Req#"/>
     <tableColumn id="3" name="Category"/>
     <tableColumn id="4" name="Description"/>
@@ -407,7 +447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10:D11"/>
     </sheetView>
   </sheetViews>
@@ -508,4 +548,114 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="211.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E49">
+      <formula1>"FUNC,NON-FUNC"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:C49">
+      <formula1>"Open,Done"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Minor updates to finitestatemachine class to remove forced overload of various functions
</commit_message>
<xml_diff>
--- a/SRS/requirements.xlsx
+++ b/SRS/requirements.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>Status</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Trading prices shall add zeros such that all data has the same string length (i.e: "1000.25,1005,1000.50,900,500.005" shall be coded as "1000.250,1005.000,1000.500,500.005"</t>
+  </si>
+  <si>
+    <t>Upon connection, all available trading instruments shall update their stored data file</t>
   </si>
 </sst>
 </file>
@@ -552,10 +555,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,6 +641,14 @@
       </c>
       <c r="F7" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>